<commit_message>
add two rows to templates/DailyReport-Potentia
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-Potentia.xlsx
+++ b/job/templates/DailyReport-Potentia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20280" windowHeight="12240"/>
+    <workbookView windowWidth="28800" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProductionReport" sheetId="1" r:id="rId1"/>
@@ -127,13 +127,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-10409]#,##0;\(#,##0\)"/>
-    <numFmt numFmtId="178" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
-    <numFmt numFmtId="179" formatCode="0.0%"/>
-    <numFmt numFmtId="180" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-10409]#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="179" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="180" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="181" formatCode="0.0%"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -187,6 +187,89 @@
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -197,6 +280,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -205,126 +311,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,11 +320,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -385,61 +385,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,121 +565,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,8 +957,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -981,23 +996,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1026,21 +1041,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1054,10 +1054,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1070,130 +1070,130 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="31" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,19 +1289,19 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="179" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="180" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1313,19 +1313,19 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="179" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="180" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1341,7 +1341,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1374,7 +1374,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1382,19 +1386,19 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="2" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="5" fillId="2" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1402,15 +1406,15 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1418,19 +1422,15 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="5" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1443,11 +1443,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="5" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="5" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="5" fillId="5" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="5" fillId="5" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1800,7 +1800,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2028,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="49" t="e">
-        <f>J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K13" si="0">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="48">
@@ -2066,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="49" t="e">
-        <f>J11*(M11/L11)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="48">
@@ -2090,113 +2090,189 @@
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:18">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="48">
         <f>F12/$R$3</f>
         <v>0</v>
       </c>
-      <c r="K12" s="54" t="e">
-        <f>J12*(M12/L12)</f>
+      <c r="K12" s="49" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="48">
         <f>G12/$R$3</f>
         <v>0</v>
       </c>
-      <c r="M12" s="55"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
       <c r="P12" s="51" t="e">
         <f>I12/(J12*$R$4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="66" t="e">
+      <c r="Q12" s="65" t="e">
         <f>I12/((F12/$R$3*$R$4)*R12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="66" t="e">
+      <c r="R12" s="65" t="e">
         <f>H12/(L12*$R$4)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" ht="13.15" customHeight="1" spans="1:19">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38">
-        <f t="shared" ref="D13:N13" si="0">SUM(D10:D12)</f>
+    <row r="13" customHeight="1" spans="1:18">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="48">
+        <f>F13/$R$3</f>
         <v>0</v>
       </c>
-      <c r="E13" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="58" t="e">
+      <c r="K13" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L13" s="58">
-        <f t="shared" si="0"/>
+      <c r="L13" s="48">
+        <f>G13/$R$3</f>
         <v>0</v>
       </c>
-      <c r="M13" s="59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61" t="e">
+      <c r="M13" s="50"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="51" t="e">
         <f>I13/(J13*$R$4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q13" s="61" t="e">
+      <c r="Q13" s="65" t="e">
         <f>I13/((F13/$R$3*$R$4)*R13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="61" t="e">
+      <c r="R13" s="65" t="e">
         <f>H13/(L13*$R$4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S13" s="67"/>
     </row>
-    <row r="16" customHeight="1" spans="3:3">
-      <c r="C16" s="39"/>
+    <row r="14" customHeight="1" spans="1:18">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53">
+        <f>F14/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="54" t="e">
+        <f>J14*(M14/L14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" s="53">
+        <f>G14/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="55"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="51" t="e">
+        <f>I14/(J14*$R$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q14" s="66" t="e">
+        <f>I14/((F14/$R$3*$R$4)*R14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="66" t="e">
+        <f>H14/(L14*$R$4)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="17" customHeight="1" spans="3:3">
-      <c r="C17" s="39"/>
+    <row r="15" ht="13.15" customHeight="1" spans="1:19">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38">
+        <f t="shared" ref="D15:N15" si="1">SUM(D10:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="58" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="60"/>
+      <c r="P15" s="61" t="e">
+        <f>I15/(J15*$R$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q15" s="61" t="e">
+        <f>I15/((F15/$R$3*$R$4)*R15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" s="61" t="e">
+        <f>H15/(L15*$R$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S15" s="67"/>
+    </row>
+    <row r="18" customHeight="1" spans="3:3">
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" customHeight="1" spans="3:3">
+      <c r="C19" s="39"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2217,8 +2293,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="I13" formula="1" unlockedFormula="1"/>
-    <ignoredError sqref="D13:H13 K11 K10 J13:N13" unlockedFormula="1"/>
+    <ignoredError sqref="I15" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="J15:N15 K10 K11 D15:H15" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>